<commit_message>
Incorporate I/O files from RMI
</commit_message>
<xml_diff>
--- a/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
+++ b/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
@@ -1,41 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\io-model\BECbIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\io-model\BECbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B79BD9-20AC-45FF-A8C3-5DA680E41FFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5445"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="OECD VAL" sheetId="7" r:id="rId2"/>
-    <sheet name="BECbIC" sheetId="2" r:id="rId3"/>
+    <sheet name="OECD VAL" sheetId="2" r:id="rId2"/>
+    <sheet name="BECbIC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+  <si>
+    <t>BECbIC BAU Employee Compensation by ISIC Code</t>
+  </si>
   <si>
     <t>Source:</t>
   </si>
@@ -43,12 +32,42 @@
     <t>OECD</t>
   </si>
   <si>
+    <t>Input-Output Tables 2018 Edition (ISIC Rev. 4)</t>
+  </si>
+  <si>
+    <t>https://stats.oecd.org/Index.aspx?DataSetCode=IOTS#</t>
+  </si>
+  <si>
+    <t>Variable: VAL</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
+    <t>In the OECD dataset, employee compensation includes not just salary and bonuses</t>
+  </si>
+  <si>
+    <t>but also employer-paid benefits and employer-paid retirement plan contributions.</t>
+  </si>
+  <si>
+    <t>We convert 2015 USD to 2012 USD with the following conversion factor:</t>
+  </si>
+  <si>
+    <t>2012 USD per 2015 USD</t>
+  </si>
+  <si>
     <t>Sorry, the query is too large to fit into the Excel cell. You will not be able to update your table with the .Stat Populator.</t>
   </si>
   <si>
+    <t>Dataset: Input-Output Tables 2018 edition</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>VAL: Value added</t>
+  </si>
+  <si>
     <t>Country</t>
   </si>
   <si>
@@ -64,7 +83,136 @@
     <t>Unit</t>
   </si>
   <si>
-    <t/>
+    <t>US Dollar, Millions</t>
+  </si>
+  <si>
+    <t>To: (sector in column)</t>
+  </si>
+  <si>
+    <t>D01T03: Agriculture, forestry and fishing</t>
+  </si>
+  <si>
+    <t>D05T06: Mining and extraction of energy producing products</t>
+  </si>
+  <si>
+    <t>D07T08: Mining and quarrying of non-energy producing products</t>
+  </si>
+  <si>
+    <t>D09: Mining support service activities</t>
+  </si>
+  <si>
+    <t>D10T12: Food products, beverages and tobacco</t>
+  </si>
+  <si>
+    <t>D13T15: Textiles, wearing apparel, leather and related products</t>
+  </si>
+  <si>
+    <t>D16: Wood and products of wood and cork</t>
+  </si>
+  <si>
+    <t>D17T18: Paper products and printing</t>
+  </si>
+  <si>
+    <t>D19: Coke and refined petroleum products</t>
+  </si>
+  <si>
+    <t>D20T21: Chemicals and pharmaceutical products</t>
+  </si>
+  <si>
+    <t>D22: Rubber and plastic products</t>
+  </si>
+  <si>
+    <t>D23: Other non-metallic mineral products</t>
+  </si>
+  <si>
+    <t>D24: Basic metals</t>
+  </si>
+  <si>
+    <t>D25: Fabricated metal products</t>
+  </si>
+  <si>
+    <t>D26: Computer, electronic and optical products</t>
+  </si>
+  <si>
+    <t>D27: Electrical equipment</t>
+  </si>
+  <si>
+    <t>D28: Machinery and equipment, nec</t>
+  </si>
+  <si>
+    <t>D29: Motor vehicles, trailers and semi-trailers</t>
+  </si>
+  <si>
+    <t>D30: Other transport equipment</t>
+  </si>
+  <si>
+    <t>D31T33: Other manufacturing; repair and installation of machinery and equipment</t>
+  </si>
+  <si>
+    <t>D35T39: Electricity, gas, water supply, sewerage, waste and remediation services</t>
+  </si>
+  <si>
+    <t>D41T43: Construction</t>
+  </si>
+  <si>
+    <t>D45T47: Wholesale and retail trade; repair of motor vehicles</t>
+  </si>
+  <si>
+    <t>D49T53: Transportation and storage</t>
+  </si>
+  <si>
+    <t>D55T56: Accomodation and food services</t>
+  </si>
+  <si>
+    <t>D58T60: Publishing, audiovisual and broadcasting activities</t>
+  </si>
+  <si>
+    <t>D61: Telecommunications</t>
+  </si>
+  <si>
+    <t>D62T63: IT and other information services</t>
+  </si>
+  <si>
+    <t>D64T66: Financial and insurance activities</t>
+  </si>
+  <si>
+    <t>D68: Real estate activities</t>
+  </si>
+  <si>
+    <t>D69T82: Other business sector services</t>
+  </si>
+  <si>
+    <t>D84: Public admin. and defence; compulsory social security</t>
+  </si>
+  <si>
+    <t>D85: Education</t>
+  </si>
+  <si>
+    <t>D86T88: Human health and social work</t>
+  </si>
+  <si>
+    <t>D90T96: Arts, entertainment, recreation and other service activities</t>
+  </si>
+  <si>
+    <t>D97T98: Private households with employed persons</t>
+  </si>
+  <si>
+    <t>From: (sector in row)</t>
+  </si>
+  <si>
+    <t>LABR: Compensation of employees</t>
+  </si>
+  <si>
+    <t>OTXS: Other taxes less subsidies on production</t>
+  </si>
+  <si>
+    <t>GOPS: Gross operating surplus and mixed income</t>
+  </si>
+  <si>
+    <t>Data extracted on 03 Jun 2020 20:52 UTC (GMT) from OECD.Stat</t>
+  </si>
+  <si>
+    <t>Unit: $</t>
   </si>
   <si>
     <t>ISIC 01T03</t>
@@ -175,178 +323,13 @@
     <t>ISIC 97T98</t>
   </si>
   <si>
-    <t>https://stats.oecd.org/Index.aspx?DataSetCode=IOTS#</t>
-  </si>
-  <si>
-    <t>Dataset: Input-Output Tables 2018 edition</t>
-  </si>
-  <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>VAL: Value added</t>
-  </si>
-  <si>
-    <t>US Dollar, Millions</t>
-  </si>
-  <si>
-    <t>To: (sector in column)</t>
-  </si>
-  <si>
-    <t>D01T03: Agriculture, forestry and fishing</t>
-  </si>
-  <si>
-    <t>D05T06: Mining and extraction of energy producing products</t>
-  </si>
-  <si>
-    <t>D07T08: Mining and quarrying of non-energy producing products</t>
-  </si>
-  <si>
-    <t>D09: Mining support service activities</t>
-  </si>
-  <si>
-    <t>D10T12: Food products, beverages and tobacco</t>
-  </si>
-  <si>
-    <t>D13T15: Textiles, wearing apparel, leather and related products</t>
-  </si>
-  <si>
-    <t>D16: Wood and products of wood and cork</t>
-  </si>
-  <si>
-    <t>D17T18: Paper products and printing</t>
-  </si>
-  <si>
-    <t>D19: Coke and refined petroleum products</t>
-  </si>
-  <si>
-    <t>D20T21: Chemicals and pharmaceutical products</t>
-  </si>
-  <si>
-    <t>D22: Rubber and plastic products</t>
-  </si>
-  <si>
-    <t>D23: Other non-metallic mineral products</t>
-  </si>
-  <si>
-    <t>D24: Basic metals</t>
-  </si>
-  <si>
-    <t>D25: Fabricated metal products</t>
-  </si>
-  <si>
-    <t>D26: Computer, electronic and optical products</t>
-  </si>
-  <si>
-    <t>D27: Electrical equipment</t>
-  </si>
-  <si>
-    <t>D28: Machinery and equipment, nec</t>
-  </si>
-  <si>
-    <t>D29: Motor vehicles, trailers and semi-trailers</t>
-  </si>
-  <si>
-    <t>D30: Other transport equipment</t>
-  </si>
-  <si>
-    <t>D31T33: Other manufacturing; repair and installation of machinery and equipment</t>
-  </si>
-  <si>
-    <t>D35T39: Electricity, gas, water supply, sewerage, waste and remediation services</t>
-  </si>
-  <si>
-    <t>D41T43: Construction</t>
-  </si>
-  <si>
-    <t>D45T47: Wholesale and retail trade; repair of motor vehicles</t>
-  </si>
-  <si>
-    <t>D49T53: Transportation and storage</t>
-  </si>
-  <si>
-    <t>D55T56: Accomodation and food services</t>
-  </si>
-  <si>
-    <t>D58T60: Publishing, audiovisual and broadcasting activities</t>
-  </si>
-  <si>
-    <t>D61: Telecommunications</t>
-  </si>
-  <si>
-    <t>D62T63: IT and other information services</t>
-  </si>
-  <si>
-    <t>D64T66: Financial and insurance activities</t>
-  </si>
-  <si>
-    <t>D68: Real estate activities</t>
-  </si>
-  <si>
-    <t>D69T82: Other business sector services</t>
-  </si>
-  <si>
-    <t>D84: Public admin. and defence; compulsory social security</t>
-  </si>
-  <si>
-    <t>D85: Education</t>
-  </si>
-  <si>
-    <t>D86T88: Human health and social work</t>
-  </si>
-  <si>
-    <t>D90T96: Arts, entertainment, recreation and other service activities</t>
-  </si>
-  <si>
-    <t>D97T98: Private households with employed persons</t>
-  </si>
-  <si>
-    <t>From: (sector in row)</t>
-  </si>
-  <si>
-    <t>LABR: Compensation of employees</t>
-  </si>
-  <si>
-    <t>OTXS: Other taxes less subsidies on production</t>
-  </si>
-  <si>
-    <t>GOPS: Gross operating surplus and mixed income</t>
-  </si>
-  <si>
-    <t>Data extracted on 03 Jun 2020 20:52 UTC (GMT) from OECD.Stat</t>
-  </si>
-  <si>
     <t>Employee Compensation</t>
-  </si>
-  <si>
-    <t>Unit: $</t>
-  </si>
-  <si>
-    <t>Input-Output Tables 2018 Edition (ISIC Rev. 4)</t>
-  </si>
-  <si>
-    <t>Variable: VAL</t>
-  </si>
-  <si>
-    <t>In the OECD dataset, employee compensation includes not just salary and bonuses</t>
-  </si>
-  <si>
-    <t>but also employer-paid benefits and employer-paid retirement plan contributions.</t>
-  </si>
-  <si>
-    <t>We convert 2015 USD to 2012 USD with the following conversion factor:</t>
-  </si>
-  <si>
-    <t>2012 USD per 2015 USD</t>
-  </si>
-  <si>
-    <t>BECbIC BAU Employee Compensation by ISIC Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -484,7 +467,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -499,19 +482,6 @@
       <right style="thin">
         <color rgb="FFC0C0C0"/>
       </right>
-      <top style="thin">
-        <color rgb="FFC0C0C0"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFC0C0C0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC0C0C0"/>
-      </left>
-      <right/>
       <top style="thin">
         <color rgb="FFC0C0C0"/>
       </top>
@@ -547,10 +517,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -590,41 +560,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{3ADF3FF5-E4D2-4BC8-9960-7408DCCB591E}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -901,173 +855,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="77.5703125" customWidth="1"/>
+    <col min="2" max="2" width="77.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="16">
         <v>0.9686815713640794</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="https://stats.oecd.org/Index.aspx?DataSetCode=IOTS" xr:uid="{C45F7FD1-E582-4900-94D0-FDF23F149E19}"/>
+    <hyperlink ref="B6" r:id="rId1" display="https://stats.oecd.org/Index.aspx?DataSetCode=IOTS"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDFB116-01EC-4BC2-9D61-4219A6E9217A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL12"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="2.42578125" style="6" customWidth="1"/>
-    <col min="3" max="24" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="31" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="27.46484375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="2.46484375" style="6" customWidth="1"/>
+    <col min="3" max="24" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.46484375" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="31" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="9.46484375" style="6" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.46484375" style="6" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="9.1328125" style="6" customWidth="1"/>
+    <col min="41" max="16384" width="9.1328125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" hidden="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="e">
         <f ca="1">DotStatQuery(B1)</f>
         <v>#NAME?</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" ht="23.25" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B3" s="18"/>
-      <c r="C3" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="26"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="C3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="18"/>
+    </row>
+    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="17" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="19" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -1103,15 +1058,15 @@
       <c r="AI4" s="20"/>
       <c r="AJ4" s="20"/>
       <c r="AK4" s="20"/>
-      <c r="AL4" s="21"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AL4" s="18"/>
+    </row>
+    <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="17" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="19" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -1147,15 +1102,15 @@
       <c r="AI5" s="20"/>
       <c r="AJ5" s="20"/>
       <c r="AK5" s="20"/>
-      <c r="AL5" s="21"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="AL5" s="18"/>
+    </row>
+    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="17" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="19" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -1191,245 +1146,169 @@
       <c r="AI6" s="20"/>
       <c r="AJ6" s="20"/>
       <c r="AK6" s="20"/>
-      <c r="AL6" s="21"/>
-    </row>
-    <row r="7" spans="1:38" ht="126" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="AL6" s="18"/>
+    </row>
+    <row r="7" spans="1:38" ht="126" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="8" t="s">
+      <c r="AG7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="AH7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="AI7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="AJ7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="AK7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="AL7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="8" t="s">
+    </row>
+    <row r="8" spans="1:38" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="10"/>
+      <c r="AJ8" s="10"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
+    </row>
+    <row r="9" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="W7" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="X7" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z7" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA7" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB7" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC7" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD7" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE7" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF7" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG7" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH7" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI7" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ7" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL7" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="T8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="V8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="X8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AK8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL8" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="B9" s="10"/>
       <c r="C9" s="12">
         <v>55762.913999999997</v>
       </c>
@@ -1539,13 +1418,11 @@
         <v>21351.7</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>9</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B10" s="10"/>
       <c r="C10" s="13">
         <v>11926.959000000001</v>
       </c>
@@ -1655,13 +1532,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>9</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B11" s="10"/>
       <c r="C11" s="12">
         <v>126190.226</v>
       </c>
@@ -1771,9 +1646,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1789,9 +1664,9 @@
     <mergeCell ref="C5:AL5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=IOTSI4_2018&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{7A9908BF-E2DD-4D69-BCE4-1F9CB14D94BB}"/>
-    <hyperlink ref="C3" r:id="rId2" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=IOTSI4_2018&amp;Coords=[VAR].[VAL]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{0966C450-36F9-4126-A82E-9D08BE3AF7A9}"/>
-    <hyperlink ref="A12" r:id="rId3" display="https://stats-3.oecd.org/index.aspx?DatasetCode=IOTSI4_2018" xr:uid="{1C840AFB-BA5E-4F85-81DB-82D64D9AAE22}"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=IOTSI4_2018&amp;ShowOnWeb=true&amp;Lang=en"/>
+    <hyperlink ref="C3" r:id="rId2" display="http://localhost/OECDStat_Metadata/ShowMetadata.ashx?Dataset=IOTSI4_2018&amp;Coords=[VAR].[VAL]&amp;ShowOnWeb=true&amp;Lang=en"/>
+    <hyperlink ref="A12" r:id="rId3" display="https://stats-3.oecd.org/index.aspx?DatasetCode=IOTSI4_2018"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1799,284 +1674,250 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="37" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.796875" customWidth="1"/>
+    <col min="2" max="37" width="10.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="AG1" s="4" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="AH1" s="4" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="AJ1" s="4" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="AK1" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B2">
-        <f>'OECD VAL'!C9*10^6*About!$A$14</f>
-        <v>54016507157.360023</v>
+        <v>419602000</v>
       </c>
       <c r="C2">
-        <f>'OECD VAL'!D9*10^6*About!$A$14</f>
-        <v>42087940459.502907</v>
+        <v>538087000</v>
       </c>
       <c r="D2">
-        <f>'OECD VAL'!E9*10^6*About!$A$14</f>
-        <v>13192667088.040098</v>
+        <v>3076000</v>
       </c>
       <c r="E2">
-        <f>'OECD VAL'!F9*10^6*About!$A$14</f>
-        <v>31699803162.920803</v>
+        <v>73236000</v>
       </c>
       <c r="F2">
-        <f>'OECD VAL'!G9*10^6*About!$A$14</f>
-        <v>104565156568.91278</v>
+        <v>3486875000</v>
       </c>
       <c r="G2">
-        <f>'OECD VAL'!H9*10^6*About!$A$14</f>
-        <v>19249581096.571133</v>
+        <v>293945000</v>
       </c>
       <c r="H2">
-        <f>'OECD VAL'!I9*10^6*About!$A$14</f>
-        <v>19084921697.025951</v>
+        <v>928553000</v>
       </c>
       <c r="I2">
-        <f>'OECD VAL'!J9*10^6*About!$A$14</f>
-        <v>53950867356.721252</v>
+        <v>1641680000</v>
       </c>
       <c r="J2">
-        <f>'OECD VAL'!K9*10^6*About!$A$14</f>
-        <v>17895825352.232121</v>
+        <v>48826000</v>
       </c>
       <c r="K2">
-        <f>'OECD VAL'!L9*10^6*About!$A$14</f>
-        <v>97892958305.927429</v>
+        <v>2126406000</v>
       </c>
       <c r="L2">
-        <f>'OECD VAL'!M9*10^6*About!$A$14</f>
-        <v>48035143530.62439</v>
+        <v>1576992000</v>
       </c>
       <c r="M2">
-        <f>'OECD VAL'!N9*10^6*About!$A$14</f>
-        <v>27963696179.008259</v>
+        <v>922315000</v>
       </c>
       <c r="N2">
-        <f>'OECD VAL'!O9*10^6*About!$A$14</f>
-        <v>30535090470.641346</v>
+        <v>286641000</v>
       </c>
       <c r="O2">
-        <f>'OECD VAL'!P9*10^6*About!$A$14</f>
-        <v>93149679188.412643</v>
+        <v>1949360000</v>
       </c>
       <c r="P2">
-        <f>'OECD VAL'!Q9*10^6*About!$A$14</f>
-        <v>133807960921.68916</v>
+        <v>1691201000</v>
       </c>
       <c r="Q2">
-        <f>'OECD VAL'!R9*10^6*About!$A$14</f>
-        <v>33053576343.528103</v>
+        <v>739567000</v>
       </c>
       <c r="R2">
-        <f>'OECD VAL'!S9*10^6*About!$A$14</f>
-        <v>87657629558.546432</v>
+        <v>1800105000</v>
       </c>
       <c r="S2">
-        <f>'OECD VAL'!T9*10^6*About!$A$14</f>
-        <v>66099176562.997589</v>
+        <v>133939000</v>
       </c>
       <c r="T2">
-        <f>'OECD VAL'!U9*10^6*About!$A$14</f>
-        <v>76755469135.572556</v>
+        <v>4700050000</v>
       </c>
       <c r="U2">
-        <f>'OECD VAL'!V9*10^6*About!$A$14</f>
-        <v>70758876865.8535</v>
+        <v>879359000</v>
       </c>
       <c r="V2">
-        <f>'OECD VAL'!W9*10^6*About!$A$14</f>
-        <v>99649765984.524323</v>
+        <v>3282159000</v>
       </c>
       <c r="W2">
-        <f>'OECD VAL'!X9*10^6*About!$A$14</f>
-        <v>443551633131.10876</v>
+        <v>21614536000</v>
       </c>
       <c r="X2">
-        <f>'OECD VAL'!Y9*10^6*About!$A$14</f>
-        <v>1092867487465.397</v>
+        <v>15352128000</v>
       </c>
       <c r="Y2">
-        <f>'OECD VAL'!Z9*10^6*About!$A$14</f>
-        <v>358730084291.4812</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <f>'OECD VAL'!AA9*10^6*About!$A$14</f>
-        <v>330227698478.54797</v>
+        <v>13649840000</v>
       </c>
       <c r="AA2">
-        <f>'OECD VAL'!AB9*10^6*About!$A$14</f>
-        <v>197642858841.8468</v>
+        <v>6848602000</v>
       </c>
       <c r="AB2">
-        <f>'OECD VAL'!AC9*10^6*About!$A$14</f>
-        <v>83292175969.808075</v>
+        <v>6375142000</v>
       </c>
       <c r="AC2">
-        <f>'OECD VAL'!AD9*10^6*About!$A$14</f>
-        <v>286458782608.58081</v>
+        <v>6917900000</v>
       </c>
       <c r="AD2">
-        <f>'OECD VAL'!AE9*10^6*About!$A$14</f>
-        <v>726862913582.39282</v>
+        <v>30996753000</v>
       </c>
       <c r="AE2">
-        <f>'OECD VAL'!AF9*10^6*About!$A$14</f>
-        <v>99124994367.416687</v>
+        <v>6275096000</v>
       </c>
       <c r="AF2">
-        <f>'OECD VAL'!AG9*10^6*About!$A$14</f>
-        <v>1320219395505.2676</v>
+        <v>144745679000</v>
       </c>
       <c r="AG2">
-        <f>'OECD VAL'!AH9*10^6*About!$A$14</f>
-        <v>1182871631888.7844</v>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <f>'OECD VAL'!AI9*10^6*About!$A$14</f>
-        <v>838587376723.22241</v>
+        <v>5880523000</v>
       </c>
       <c r="AI2">
-        <f>'OECD VAL'!AJ9*10^6*About!$A$14</f>
-        <v>1041787952118.6583</v>
+        <v>47700592000</v>
       </c>
       <c r="AJ2">
-        <f>'OECD VAL'!AK9*10^6*About!$A$14</f>
-        <v>309954904850.23438</v>
+        <v>3127186000</v>
       </c>
       <c r="AK2">
-        <f>'OECD VAL'!AL9*10^6*About!$A$14</f>
-        <v>20682998307.294415</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RMI's edited employment files
</commit_message>
<xml_diff>
--- a/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
+++ b/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
@@ -1720,112 +1720,112 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>215724000</v>
+        <v>334498000</v>
       </c>
       <c r="C2" t="n">
-        <v>299912000</v>
+        <v>30498000</v>
       </c>
       <c r="D2" t="n">
-        <v>3076000</v>
+        <v>455922000</v>
       </c>
       <c r="E2" t="n">
-        <v>44342000</v>
+        <v>60905000</v>
       </c>
       <c r="F2" t="n">
-        <v>1832343000</v>
+        <v>2524372000</v>
       </c>
       <c r="G2" t="n">
-        <v>243795000</v>
+        <v>385940000</v>
       </c>
       <c r="H2" t="n">
-        <v>529490000</v>
+        <v>755317000</v>
       </c>
       <c r="I2" t="n">
-        <v>986654000</v>
+        <v>1249502000</v>
       </c>
       <c r="J2" t="n">
-        <v>46736000</v>
+        <v>57723000</v>
       </c>
       <c r="K2" t="n">
-        <v>1215908000</v>
+        <v>1620819000</v>
       </c>
       <c r="L2" t="n">
-        <v>960225000</v>
+        <v>1198491000</v>
       </c>
       <c r="M2" t="n">
-        <v>515041000</v>
+        <v>588329000</v>
       </c>
       <c r="N2" t="n">
-        <v>244099000</v>
+        <v>330884000</v>
       </c>
       <c r="O2" t="n">
-        <v>996628000</v>
+        <v>1381440000</v>
       </c>
       <c r="P2" t="n">
-        <v>875881000</v>
+        <v>1648262000</v>
       </c>
       <c r="Q2" t="n">
-        <v>457764000</v>
+        <v>748548000</v>
       </c>
       <c r="R2" t="n">
-        <v>948985000</v>
+        <v>1164066000</v>
       </c>
       <c r="S2" t="n">
-        <v>133939000</v>
+        <v>1899830000</v>
       </c>
       <c r="T2" t="n">
-        <v>2645101000</v>
+        <v>1899830000</v>
       </c>
       <c r="U2" t="n">
-        <v>491425000</v>
+        <v>696553000</v>
       </c>
       <c r="V2" t="n">
-        <v>1733896000</v>
+        <v>1750195000</v>
       </c>
       <c r="W2" t="n">
-        <v>10807268000</v>
+        <v>14034882000</v>
       </c>
       <c r="X2" t="n">
-        <v>7678124000</v>
+        <v>25994425000</v>
       </c>
       <c r="Y2" t="n">
-        <v>0</v>
+        <v>8380872000</v>
       </c>
       <c r="Z2" t="n">
-        <v>6826196000</v>
+        <v>9204917000</v>
       </c>
       <c r="AA2" t="n">
-        <v>3445194000</v>
+        <v>4292259000</v>
       </c>
       <c r="AB2" t="n">
-        <v>3197219000</v>
+        <v>3419210000</v>
       </c>
       <c r="AC2" t="n">
-        <v>3479268000</v>
+        <v>1605057000</v>
       </c>
       <c r="AD2" t="n">
-        <v>15498661000</v>
+        <v>17367732000</v>
       </c>
       <c r="AE2" t="n">
-        <v>3137829000</v>
+        <v>3789368000</v>
       </c>
       <c r="AF2" t="n">
-        <v>72456911000</v>
+        <v>9936572000</v>
       </c>
       <c r="AG2" t="n">
-        <v>0</v>
+        <v>78479300000</v>
       </c>
       <c r="AH2" t="n">
-        <v>2951540000</v>
+        <v>3888187000</v>
       </c>
       <c r="AI2" t="n">
-        <v>23852637000</v>
+        <v>28121793000</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1564707000</v>
+        <v>2028125000</v>
       </c>
       <c r="AK2" t="n">
-        <v>0</v>
+        <v>616910000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>